<commit_message>
Components added and first schematic drawn
</commit_message>
<xml_diff>
--- a/Window calculations.xlsx
+++ b/Window calculations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielAlvarez\Desktop\Power board\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielAlvarez\Desktop\Power board\Window_Comparator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5D3F8F7-D211-49EB-8376-A56C84B1A3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6798A05F-164D-4AF8-BDE0-6965C4567752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{420D4E37-EA78-46E9-A762-04986C5781A3}"/>
   </bookViews>
@@ -32,6 +32,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -417,7 +428,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E2" activeCellId="1" sqref="E6 E2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -447,7 +458,7 @@
         <v>2</v>
       </c>
       <c r="H2">
-        <v>5000</v>
+        <v>6800</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -483,14 +494,14 @@
         <v>0</v>
       </c>
       <c r="B6" s="1">
-        <v>200000</v>
+        <v>120000</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
       </c>
       <c r="H6">
         <f>rtotal2/r_3_2*vit</f>
-        <v>80</v>
+        <v>58.82352941176471</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -499,14 +510,14 @@
       </c>
       <c r="B7">
         <f>rtotal/vov*vit</f>
-        <v>8000</v>
+        <v>4800</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
       </c>
       <c r="H7">
         <f>vit*rtotal2/(r_2_2+r_3_2)</f>
-        <v>80</v>
+        <v>58.823529411764703</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -515,7 +526,7 @@
       </c>
       <c r="B8">
         <f>(rtotal/vuv*vit)-r_3</f>
-        <v>333.33333333333394</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -524,7 +535,7 @@
       </c>
       <c r="B9">
         <f>rtotal-r_2-r_3</f>
-        <v>191666.66666666666</v>
+        <v>115000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>